<commit_message>
Changed class name from NNLayer to Layer.
</commit_message>
<xml_diff>
--- a/NN/NeuralNet Calc.xlsx
+++ b/NN/NeuralNet Calc.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="28705"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="37440" windowHeight="16120" tabRatio="308"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38320" windowHeight="17340" tabRatio="308"/>
   </bookViews>
   <sheets>
     <sheet name="sample-1 BETTER" sheetId="19" r:id="rId1"/>
@@ -2615,7 +2615,7 @@
   <dimension ref="A1:BG23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J3" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="AH12" sqref="AH12"/>
+      <selection activeCell="AO22" sqref="AO22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>